<commit_message>
modified:   Data.xlsx 	modified:   __pycache__/app.cpython-39.pyc 	modified:   app.py 	modified:   instance/db.db 	modified:   static/my_override_style.css 	modified:   templates/reads_history.html 	modified:   templates/reads_stats.html 	modified:   templates/runs_history.html 	modified:   templates/runs_new.html
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhsengland-my.sharepoint.com/personal/andrew_pike9_england_nhs_uk/Documents/Desktop/NHS England/Personal/Andy Site/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{7ACF4993-8E2D-4DBE-AE4F-61FF9DB71A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C7CC006-120D-4CE5-9CF4-FFC1E386E48C}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{7ACF4993-8E2D-4DBE-AE4F-61FF9DB71A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E8FB4B7-93D0-4EAF-AE95-4995E88DBE2F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{7FE89C6B-0D6B-49AE-9239-99156FA3D800}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>home</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Date End - Date Start</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Blob</t>
   </si>
 </sst>
 </file>
@@ -238,13 +244,7 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -253,6 +253,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,11 +604,11 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -682,34 +688,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1140BDB1-0EE0-42B5-B05A-EB8B94FE79F6}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="3" width="14.54296875" style="3" customWidth="1"/>
+    <col min="2" max="3" width="14.54296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -717,10 +723,10 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -728,7 +734,7 @@
       <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -736,7 +742,7 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -744,54 +750,54 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -799,10 +805,10 @@
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -810,7 +816,7 @@
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -818,7 +824,7 @@
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -826,7 +832,7 @@
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -834,10 +840,10 @@
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -845,7 +851,7 @@
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -853,7 +859,7 @@
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -861,156 +867,164 @@
       <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="B34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1018,8 +1032,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>